<commit_message>
update unittest code: test_log.py, test_validator.py;
update README file of Framework_unittest;

modify unittest excel
</commit_message>
<xml_diff>
--- a/Test_Plan/Loaded_TEST_PLAN_unittest.xlsx
+++ b/Test_Plan/Loaded_TEST_PLAN_unittest.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12648" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="config" sheetId="1" state="visible" r:id="rId1"/>
@@ -112,8 +112,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="3" displayName="Table2" headerRowCount="1" headerRowDxfId="4" id="2" name="Table2" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="3" displayName="Table2" headerRowCount="1" headerRowDxfId="4" id="2" name="Table2" ref="A1:C2" totalsRowShown="0">
+  <autoFilter ref="A1:C2"/>
   <tableColumns count="3">
     <tableColumn dataDxfId="2" id="1" name="IP"/>
     <tableColumn dataDxfId="1" id="2" name="MAC"/>
@@ -404,7 +404,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -497,10 +497,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -544,26 +544,9 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>15.83.250.2</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>13354k31sb</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>WES7P</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="C2:C3" type="list">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="C2" type="list">
       <formula1>"WES7E,WES7P,WES10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>